<commit_message>
Added tests for FundRation, needs to be improved
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_ratios/capital_calls.xlsx
+++ b/public/sample_uploads/fund_ratios/capital_calls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b9b322f8db0eee2/Desktop/Ausang/AltConnects/Demo Inc Formats/Demo fund info/Ratios fund/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\fund_ratios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{EC915532-3F06-4D74-8884-DBC9CBC483D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BE75D68-25BA-4D21-9582-E69855CD177C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7E041E-FBFF-4722-816B-0E47050B662C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalCall" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -518,7 +516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -527,6 +525,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,23 +726,23 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.58203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.9140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.9140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.9140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.08203125" style="1" customWidth="1"/>
-    <col min="9" max="12" width="21.4140625" style="1" customWidth="1"/>
-    <col min="13" max="14" width="8.58203125" style="1"/>
+    <col min="1" max="1" width="9.5625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.8125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.8125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.9375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.9375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.9375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.8125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.0625" style="1" customWidth="1"/>
+    <col min="9" max="12" width="21.4375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="8.5625" style="1"/>
     <col min="15" max="15" width="10" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.58203125" style="1"/>
+    <col min="16" max="16384" width="8.5625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -782,7 +781,7 @@
       </c>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -792,12 +791,11 @@
       <c r="C2" s="5">
         <v>100</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="8">
+        <v>44856</v>
+      </c>
+      <c r="E2" s="6">
         <v>44870</v>
-      </c>
-      <c r="E2" s="6">
-        <f>D2+7</f>
-        <v>44877</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>12</v>
@@ -821,13 +819,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:13" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:13" ht="14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D5" s="4"/>
     </row>
   </sheetData>
@@ -855,16 +853,16 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.9140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.9375" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.4140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.4375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -889,7 +887,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -903,7 +901,7 @@
         <v>44571</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -917,7 +915,7 @@
         <v>44722</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Fixed tests for fund_units
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_ratios/capital_calls.xlsx
+++ b/public/sample_uploads/fund_ratios/capital_calls.xlsx
@@ -5,17 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\fund_ratios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f10f76f200b1328/Desktop/ratios auto test/bulk files/fund 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7E041E-FBFF-4722-816B-0E47050B662C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{C5D11951-2321-490A-9F77-758B5085BB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2210010-36AA-43FD-B7E4-F5E4EB12AFC1}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalCall" sheetId="1" r:id="rId1"/>
     <sheet name="Exchange Rates" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CapitalCall!$A$1:$O$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -26,6 +29,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -357,7 +363,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Fund *</t>
   </si>
@@ -398,6 +404,9 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>All</t>
+  </si>
+  <si>
     <t>Percentage of Commitment</t>
   </si>
   <si>
@@ -416,22 +425,16 @@
     <t>As Of</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>INR</t>
-  </si>
-  <si>
-    <t>First Close</t>
-  </si>
-  <si>
-    <t>Fund X</t>
-  </si>
-  <si>
-    <t>Drawdown 1</t>
-  </si>
-  <si>
-    <t>A:1000:0</t>
+    <t>Call 1</t>
+  </si>
+  <si>
+    <t>Call 2</t>
+  </si>
+  <si>
+    <t>A1:100:0,A2:100:0</t>
+  </si>
+  <si>
+    <t>Demo Fund 1</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -480,11 +483,6 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -512,24 +510,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{23C0DD61-BDF7-422F-9B4F-ACB3AC210E32}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -723,26 +716,26 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.8125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.8125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.9375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.9375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.9375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.8125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.0625" style="1" customWidth="1"/>
-    <col min="9" max="12" width="21.4375" style="1" customWidth="1"/>
-    <col min="13" max="14" width="8.5625" style="1"/>
+    <col min="1" max="1" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.125" style="1" customWidth="1"/>
+    <col min="9" max="12" width="21.375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="8.625" style="1"/>
     <col min="15" max="15" width="10" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.5625" style="1"/>
+    <col min="16" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -781,46 +774,81 @@
       </c>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45017</v>
+      </c>
+      <c r="E2" s="3">
+        <v>45026</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5">
-        <v>100</v>
-      </c>
-      <c r="D2" s="8">
-        <v>44856</v>
-      </c>
-      <c r="E2" s="6">
-        <v>44870</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45200</v>
+      </c>
+      <c r="E3" s="3">
+        <v>45209</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="D3" s="4"/>
+      <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D4" s="4"/>
@@ -830,7 +858,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 I3:L1000" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:L1000 I2:I1000" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Percentage of Commitment,Upload"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -850,30 +878,30 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.9375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.4375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -888,46 +916,13 @@
       <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1">
-        <v>80</v>
-      </c>
-      <c r="D2" s="3">
-        <v>44571</v>
-      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1">
-        <v>81</v>
-      </c>
-      <c r="D3" s="3">
-        <v>44722</v>
-      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1">
-        <v>82</v>
-      </c>
-      <c r="D4" s="3">
-        <v>44905</v>
-      </c>
+      <c r="D4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Added working test for fund ratio computation
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_ratios/capital_calls.xlsx
+++ b/public/sample_uploads/fund_ratios/capital_calls.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f10f76f200b1328/Desktop/ratios auto test/bulk files/fund 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f10f76f200b1328/Desktop/ratios auto test/bulk files/fund 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{C5D11951-2321-490A-9F77-758B5085BB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2210010-36AA-43FD-B7E4-F5E4EB12AFC1}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{C5D11951-2321-490A-9F77-758B5085BB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3332FDA-A66B-434E-85F2-AD8A809A5454}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,7 +434,7 @@
     <t>A1:100:0,A2:100:0</t>
   </si>
   <si>
-    <t>Demo Fund 1</t>
+    <t>Demo Fund 2</t>
   </si>
 </sst>
 </file>
@@ -716,7 +716,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>

</xml_diff>